<commit_message>
corrected test result and created graphs
</commit_message>
<xml_diff>
--- a/paper/sac2017/summary_1509.xlsx
+++ b/paper/sac2017/summary_1509.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 device" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="_1000k_package" localSheetId="3">'4 devices'!$N$2:$N$32</definedName>
     <definedName name="_1000k_package_1" localSheetId="2">'3 devices'!#REF!</definedName>
     <definedName name="_1000k_package_1" localSheetId="3">'4 devices'!$N$37:$N$66</definedName>
-    <definedName name="_1000k_package_2" localSheetId="2">'3 devices'!$N$65:$O$95</definedName>
+    <definedName name="_1000k_package_2" localSheetId="2">'3 devices'!$N$67:$O$97</definedName>
     <definedName name="_1000k_package_2" localSheetId="3">'4 devices'!$N$78:$N$107</definedName>
     <definedName name="_1000k_package_3" localSheetId="3">'4 devices'!$N$112:$N$139</definedName>
     <definedName name="_100k_package" localSheetId="1">'2 devices'!$F$2:$F$32</definedName>
@@ -27,7 +27,7 @@
     <definedName name="_100k_package" localSheetId="3">'4 devices'!$H$2:$I$35</definedName>
     <definedName name="_100k_package_1" localSheetId="2">'3 devices'!#REF!</definedName>
     <definedName name="_100k_package_1" localSheetId="3">'4 devices'!$X$2:$Y$63</definedName>
-    <definedName name="_100k_package_2" localSheetId="2">'3 devices'!$H$65:$H$95</definedName>
+    <definedName name="_100k_package_2" localSheetId="2">'3 devices'!$H$67:$H$97</definedName>
     <definedName name="_100k_package_2" localSheetId="3">'4 devices'!$AE$2:$AE$63</definedName>
     <definedName name="_100k_package_3" localSheetId="3">'4 devices'!$G$78:$H$107</definedName>
     <definedName name="_100k_package_4" localSheetId="3">'4 devices'!$AO$33:$AP$64</definedName>
@@ -35,9 +35,9 @@
     <definedName name="_10k_package" localSheetId="2">'3 devices'!$C$2:$C$28</definedName>
     <definedName name="_10k_package" localSheetId="3">'4 devices'!$D$2:$E$35</definedName>
     <definedName name="_10k_package_1" localSheetId="1">'2 devices'!$E$37:$F$67</definedName>
-    <definedName name="_10k_package_1" localSheetId="2">'3 devices'!$E$31:$F$61</definedName>
+    <definedName name="_10k_package_1" localSheetId="2">'3 devices'!$E$33:$F$63</definedName>
     <definedName name="_10k_package_1" localSheetId="3">'4 devices'!$T$2:$U$62</definedName>
-    <definedName name="_10k_package_2" localSheetId="2">'3 devices'!$D$65:$E$95</definedName>
+    <definedName name="_10k_package_2" localSheetId="2">'3 devices'!$D$67:$E$97</definedName>
     <definedName name="_10k_package_2" localSheetId="3">'4 devices'!$D$112:$K$158</definedName>
     <definedName name="_10k_package_3" localSheetId="3">'4 devices'!$C$78:$C$108</definedName>
     <definedName name="_10k_package_4" localSheetId="3">'4 devices'!$AJ$33:$AK$63</definedName>
@@ -47,14 +47,14 @@
     <definedName name="_1200k_package" localSheetId="3">'4 devices'!$O$2:$O$32</definedName>
     <definedName name="_1200k_package_1" localSheetId="2">'3 devices'!#REF!</definedName>
     <definedName name="_1200k_package_1" localSheetId="3">'4 devices'!#REF!</definedName>
-    <definedName name="_1200k_package_2" localSheetId="2">'3 devices'!$O$65:$O$95</definedName>
+    <definedName name="_1200k_package_2" localSheetId="2">'3 devices'!$O$67:$O$97</definedName>
     <definedName name="_1200k_package_2" localSheetId="3">'4 devices'!$BC$2:$BD$32</definedName>
     <definedName name="_1200k_package_3" localSheetId="3">'4 devices'!$O$112:$O$138</definedName>
     <definedName name="_1500k_package" localSheetId="0">'1 device'!$S$2:$T$32</definedName>
     <definedName name="_1500k_package" localSheetId="1">'2 devices'!$F$37:$K$67</definedName>
-    <definedName name="_1500k_package" localSheetId="2">'3 devices'!$A$31:$B$61</definedName>
+    <definedName name="_1500k_package" localSheetId="2">'3 devices'!$A$33:$B$63</definedName>
     <definedName name="_1500k_package" localSheetId="3">'4 devices'!$C$38:$D$68</definedName>
-    <definedName name="_1500k_package_1" localSheetId="1">'2 devices'!$Q$37:$Q$63</definedName>
+    <definedName name="_1500k_package_1" localSheetId="1">'2 devices'!$Q$37:$Q$68</definedName>
     <definedName name="_1500k_package_1" localSheetId="2">'3 devices'!#REF!</definedName>
     <definedName name="_1500k_package_1" localSheetId="3">'4 devices'!#REF!</definedName>
     <definedName name="_1500k_package_2" localSheetId="2">'3 devices'!$AI$2:$AJ$32</definedName>
@@ -62,7 +62,7 @@
     <definedName name="_1500k_package_3" localSheetId="3">'4 devices'!$AP$2:$AQ$32</definedName>
     <definedName name="_1k_package" localSheetId="0">'1 device'!$A$2:$B$62</definedName>
     <definedName name="_1k_package" localSheetId="1">'2 devices'!$B$2:$C$35</definedName>
-    <definedName name="_1k_package" localSheetId="2">'3 devices'!$B$2:$B$62</definedName>
+    <definedName name="_1k_package" localSheetId="2">'3 devices'!$B$2:$B$64</definedName>
     <definedName name="_1k_package" localSheetId="3">'4 devices'!$B$2:$C$35</definedName>
     <definedName name="_1k_package_1" localSheetId="1">'2 devices'!$T$2:$U$61</definedName>
     <definedName name="_1k_package_1" localSheetId="2">'3 devices'!$T$2:$U$61</definedName>
@@ -92,7 +92,7 @@
     <definedName name="_400k_package" localSheetId="1">'2 devices'!$I$2:$I$32</definedName>
     <definedName name="_400k_package" localSheetId="2">'3 devices'!$H$2:$H$28</definedName>
     <definedName name="_400k_package" localSheetId="3">'4 devices'!$H$2:$H$32</definedName>
-    <definedName name="_400k_package_1" localSheetId="2">'3 devices'!$H$31:$O$61</definedName>
+    <definedName name="_400k_package_1" localSheetId="2">'3 devices'!$H$33:$O$63</definedName>
     <definedName name="_400k_package_1" localSheetId="3">'4 devices'!$H$37:$H$67</definedName>
     <definedName name="_400k_package_2" localSheetId="2">'3 devices'!#REF!</definedName>
     <definedName name="_400k_package_2" localSheetId="3">'4 devices'!#REF!</definedName>
@@ -102,27 +102,27 @@
     <definedName name="_500k_package" localSheetId="2">'3 devices'!$I$2:$L$29</definedName>
     <definedName name="_500k_package" localSheetId="3">'4 devices'!$I$2:$I$32</definedName>
     <definedName name="_500k_package_1" localSheetId="1">'2 devices'!#REF!</definedName>
-    <definedName name="_500k_package_1" localSheetId="2">'3 devices'!$I$31:$I$61</definedName>
+    <definedName name="_500k_package_1" localSheetId="2">'3 devices'!$I$33:$I$63</definedName>
     <definedName name="_500k_package_1" localSheetId="3">'4 devices'!$I$37:$I$67</definedName>
-    <definedName name="_500k_package_2" localSheetId="2">'3 devices'!$I$65:$M$95</definedName>
+    <definedName name="_500k_package_2" localSheetId="2">'3 devices'!$I$67:$M$97</definedName>
     <definedName name="_500k_package_2" localSheetId="3">'4 devices'!#REF!</definedName>
     <definedName name="_500k_package_3" localSheetId="3">'4 devices'!$AY$3:$AZ$33</definedName>
     <definedName name="_50k_package" localSheetId="0">'1 device'!$G$2:$H$32</definedName>
     <definedName name="_50k_package" localSheetId="1">'2 devices'!$E$2:$E$32</definedName>
     <definedName name="_50k_package" localSheetId="2">'3 devices'!$D$2:$D$28</definedName>
     <definedName name="_50k_package" localSheetId="3">'4 devices'!$F$2:$G$35</definedName>
-    <definedName name="_50k_package_1" localSheetId="2">'3 devices'!$G$31:$G$61</definedName>
+    <definedName name="_50k_package_1" localSheetId="2">'3 devices'!$G$33:$G$63</definedName>
     <definedName name="_50k_package_1" localSheetId="3">'4 devices'!$V$2:$W$63</definedName>
-    <definedName name="_50k_package_2" localSheetId="2">'3 devices'!$F$65:$G$95</definedName>
+    <definedName name="_50k_package_2" localSheetId="2">'3 devices'!$F$67:$G$97</definedName>
     <definedName name="_50k_package_2" localSheetId="3">'4 devices'!$AD$2:$AD$63</definedName>
     <definedName name="_50k_package_3" localSheetId="3">'4 devices'!$E$78:$F$108</definedName>
     <definedName name="_600k_package" localSheetId="1">'2 devices'!$K$2:$L$32</definedName>
     <definedName name="_600k_package" localSheetId="2">'3 devices'!$J$2:$J$28</definedName>
     <definedName name="_600k_package" localSheetId="3">'4 devices'!$J$2:$K$32</definedName>
     <definedName name="_600k_package_1" localSheetId="1">'2 devices'!#REF!</definedName>
-    <definedName name="_600k_package_1" localSheetId="2">'3 devices'!$K$31:$L$61</definedName>
+    <definedName name="_600k_package_1" localSheetId="2">'3 devices'!$K$33:$L$63</definedName>
     <definedName name="_600k_package_1" localSheetId="3">'4 devices'!$J$37:$K$67</definedName>
-    <definedName name="_600k_package_2" localSheetId="2">'3 devices'!$J$65:$J$86</definedName>
+    <definedName name="_600k_package_2" localSheetId="2">'3 devices'!$J$67:$J$88</definedName>
     <definedName name="_600k_package_2" localSheetId="3">'4 devices'!$J$78:$N$108</definedName>
     <definedName name="_600k_package_3" localSheetId="3">'4 devices'!$J$112:$J$142</definedName>
     <definedName name="_700k_package" localSheetId="0">'1 device'!$AB$2:$AC$32</definedName>
@@ -130,18 +130,18 @@
     <definedName name="_700k_package" localSheetId="2">'3 devices'!$K$2:$K$29</definedName>
     <definedName name="_700k_package" localSheetId="3">'4 devices'!$K$2:$K$32</definedName>
     <definedName name="_700k_package_1" localSheetId="1">'2 devices'!$L$37:$Q$67</definedName>
-    <definedName name="_700k_package_1" localSheetId="2">'3 devices'!$M$31:$N$61</definedName>
+    <definedName name="_700k_package_1" localSheetId="2">'3 devices'!$M$33:$N$63</definedName>
     <definedName name="_700k_package_1" localSheetId="3">'4 devices'!$K$37:$K$67</definedName>
-    <definedName name="_700k_package_2" localSheetId="2">'3 devices'!$K$65:$K$94</definedName>
+    <definedName name="_700k_package_2" localSheetId="2">'3 devices'!$K$67:$K$96</definedName>
     <definedName name="_700k_package_2" localSheetId="3">'4 devices'!$K$78:$K$108</definedName>
     <definedName name="_700k_package_3" localSheetId="3">'4 devices'!$K$112:$K$135</definedName>
     <definedName name="_800k_package" localSheetId="1">'2 devices'!$O$2:$P$32</definedName>
     <definedName name="_800k_package" localSheetId="2">'3 devices'!$L$2:$L$28</definedName>
     <definedName name="_800k_package" localSheetId="3">'4 devices'!$L$2:$L$32</definedName>
     <definedName name="_800k_package_1" localSheetId="1">'2 devices'!$M$37:$M$62</definedName>
-    <definedName name="_800k_package_1" localSheetId="2">'3 devices'!$O$31:$P$61</definedName>
+    <definedName name="_800k_package_1" localSheetId="2">'3 devices'!$O$33:$P$63</definedName>
     <definedName name="_800k_package_1" localSheetId="3">'4 devices'!#REF!</definedName>
-    <definedName name="_800k_package_2" localSheetId="2">'3 devices'!$L$65:$L$93</definedName>
+    <definedName name="_800k_package_2" localSheetId="2">'3 devices'!$L$67:$L$95</definedName>
     <definedName name="_800k_package_2" localSheetId="3">'4 devices'!$L$37:$L$67</definedName>
     <definedName name="_800k_package_3" localSheetId="3">'4 devices'!$L$78:$L$108</definedName>
     <definedName name="_800k_package_4" localSheetId="3">'4 devices'!$L$112:$L$142</definedName>
@@ -1960,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3585,10 +3585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q67"/>
+  <dimension ref="B1:Q68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5146,10 +5146,6 @@
       <c r="P32" s="1">
         <v>548</v>
       </c>
-      <c r="Q32" s="2">
-        <f>AVERAGE(Q2:Q31)</f>
-        <v>663.6</v>
-      </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
@@ -5208,6 +5204,10 @@
         <f t="shared" si="0"/>
         <v>563.58064516129036</v>
       </c>
+      <c r="Q33" s="2">
+        <f>AVERAGE(Q2:Q31)</f>
+        <v>663.6</v>
+      </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -6395,9 +6395,6 @@
       <c r="P63" s="1">
         <v>1083</v>
       </c>
-      <c r="Q63" s="1">
-        <v>1864</v>
-      </c>
     </row>
     <row r="64" spans="3:17" x14ac:dyDescent="0.25">
       <c r="H64" s="1">
@@ -6407,19 +6404,81 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:17" x14ac:dyDescent="0.25">
       <c r="H65" s="1">
         <v>563</v>
       </c>
     </row>
-    <row r="66" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:17" x14ac:dyDescent="0.25">
       <c r="H66" s="1">
         <v>527</v>
       </c>
     </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:17" x14ac:dyDescent="0.25">
       <c r="H67" s="1">
         <v>782</v>
+      </c>
+    </row>
+    <row r="68" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C68" s="2">
+        <f>AVERAGE(C37:C60)</f>
+        <v>53.5</v>
+      </c>
+      <c r="D68" s="2">
+        <f>AVERAGE(D37:D60)</f>
+        <v>58.125</v>
+      </c>
+      <c r="E68" s="2">
+        <f>AVERAGE(E37:E60)</f>
+        <v>142.375</v>
+      </c>
+      <c r="F68" s="2">
+        <f>AVERAGE(F37:F60)</f>
+        <v>200.41666666666666</v>
+      </c>
+      <c r="G68" s="2">
+        <f>AVERAGE(G37:G60)</f>
+        <v>272.04166666666669</v>
+      </c>
+      <c r="H68" s="2">
+        <f>AVERAGE(H37:H67)</f>
+        <v>437.96774193548384</v>
+      </c>
+      <c r="I68" s="2">
+        <f>AVERAGE(I37:I57)</f>
+        <v>492.14285714285717</v>
+      </c>
+      <c r="J68" s="2">
+        <f>AVERAGE(J37:J53)</f>
+        <v>524.17647058823525</v>
+      </c>
+      <c r="K68" s="2">
+        <f>AVERAGE(K37:K62)</f>
+        <v>647.76923076923072</v>
+      </c>
+      <c r="L68" s="2">
+        <f>AVERAGE(L37:L59)</f>
+        <v>786.60869565217388</v>
+      </c>
+      <c r="M68" s="2">
+        <f>AVERAGE(M37:M62)</f>
+        <v>779.07692307692309</v>
+      </c>
+      <c r="N68" s="2">
+        <f>AVERAGE(N37:N60)</f>
+        <v>872.70833333333337</v>
+      </c>
+      <c r="O68" s="2">
+        <f>AVERAGE(O37:O60)</f>
+        <v>907.58333333333337</v>
+      </c>
+      <c r="P68" s="2">
+        <f>AVERAGE(P37:P64)</f>
+        <v>1130.1785714285713</v>
+      </c>
+      <c r="Q68" s="2">
+        <f>AVERAGE(Q37:Q62)</f>
+        <v>1334.4230769230769</v>
       </c>
     </row>
   </sheetData>
@@ -6430,10 +6489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q95"/>
+  <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7817,2398 +7876,2366 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <f>AVERAGE(B2:B28)</f>
+        <v>92.333333333333329</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" ref="C29:P29" si="0">AVERAGE(C2:C28)</f>
+        <v>106.48148148148148</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>162.14814814814815</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>205.11111111111111</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="0"/>
+        <v>316.77777777777777</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>437.77777777777777</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="0"/>
+        <v>508.03703703703701</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>614.03703703703707</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="0"/>
+        <v>715.74074074074076</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="0"/>
+        <v>801.59259259259261</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="0"/>
+        <v>962.74074074074076</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="0"/>
+        <v>1415.5185185185185</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="0"/>
+        <v>1150.148148148148</v>
+      </c>
+      <c r="O29" s="2">
+        <f t="shared" si="0"/>
+        <v>1238.5925925925926</v>
+      </c>
+      <c r="P29" s="2">
+        <f t="shared" si="0"/>
+        <v>1934.8888888888889</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="O32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="P32" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="1">
-        <v>27</v>
-      </c>
-      <c r="C31" s="1">
-        <v>40</v>
-      </c>
-      <c r="D31" s="1">
-        <v>146</v>
-      </c>
-      <c r="E31" s="1">
-        <v>113</v>
-      </c>
-      <c r="F31" s="1">
-        <v>186</v>
-      </c>
-      <c r="G31" s="1">
-        <v>314</v>
-      </c>
-      <c r="H31" s="1">
-        <v>218</v>
-      </c>
-      <c r="I31" s="1">
-        <v>591</v>
-      </c>
-      <c r="J31" s="1">
-        <v>263</v>
-      </c>
-      <c r="K31" s="1">
-        <v>753</v>
-      </c>
-      <c r="L31" s="1">
-        <v>485</v>
-      </c>
-      <c r="M31" s="1">
-        <v>1006</v>
-      </c>
-      <c r="N31" s="1">
-        <v>1868</v>
-      </c>
-      <c r="O31" s="1">
-        <v>1320</v>
-      </c>
-      <c r="P31" s="1">
-        <v>1451</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="1">
-        <v>35</v>
-      </c>
-      <c r="C32" s="1">
-        <v>40</v>
-      </c>
-      <c r="D32" s="1">
-        <v>148</v>
-      </c>
-      <c r="E32" s="1">
-        <v>111</v>
-      </c>
-      <c r="F32" s="1">
-        <v>150</v>
-      </c>
-      <c r="G32" s="1">
-        <v>392</v>
-      </c>
-      <c r="H32" s="1">
-        <v>537</v>
-      </c>
-      <c r="I32" s="1">
-        <v>609</v>
-      </c>
-      <c r="J32" s="1">
-        <v>270</v>
-      </c>
-      <c r="K32" s="1">
-        <v>767</v>
-      </c>
-      <c r="L32" s="1">
-        <v>422</v>
-      </c>
-      <c r="M32" s="1">
-        <v>1726</v>
-      </c>
-      <c r="N32" s="1">
-        <v>1300</v>
-      </c>
-      <c r="O32" s="1">
-        <v>1294</v>
-      </c>
-      <c r="P32" s="1">
-        <v>2601</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D33" s="1">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="E33" s="1">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F33" s="1">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G33" s="1">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="H33" s="1">
-        <v>447</v>
+        <v>218</v>
       </c>
       <c r="I33" s="1">
-        <v>533</v>
+        <v>591</v>
       </c>
       <c r="J33" s="1">
-        <v>374</v>
+        <v>263</v>
       </c>
       <c r="K33" s="1">
-        <v>775</v>
+        <v>753</v>
       </c>
       <c r="L33" s="1">
-        <v>1130</v>
+        <v>485</v>
       </c>
       <c r="M33" s="1">
-        <v>1437</v>
+        <v>1006</v>
       </c>
       <c r="N33" s="1">
-        <v>1564</v>
+        <v>1868</v>
       </c>
       <c r="O33" s="1">
-        <v>1226</v>
+        <v>1320</v>
       </c>
       <c r="P33" s="1">
-        <v>2113</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D34" s="1">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="E34" s="1">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F34" s="1">
-        <v>283</v>
+        <v>150</v>
       </c>
       <c r="G34" s="1">
-        <v>329</v>
+        <v>392</v>
       </c>
       <c r="H34" s="1">
-        <v>187</v>
+        <v>537</v>
       </c>
       <c r="I34" s="1">
-        <v>676</v>
+        <v>609</v>
       </c>
       <c r="J34" s="1">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="K34" s="1">
-        <v>647</v>
+        <v>767</v>
       </c>
       <c r="L34" s="1">
-        <v>868</v>
+        <v>422</v>
       </c>
       <c r="M34" s="1">
-        <v>1552</v>
+        <v>1726</v>
       </c>
       <c r="N34" s="1">
-        <v>1051</v>
+        <v>1300</v>
       </c>
       <c r="O34" s="1">
-        <v>1242</v>
+        <v>1294</v>
       </c>
       <c r="P34" s="1">
-        <v>1782</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D35" s="1">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E35" s="1">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="F35" s="1">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="G35" s="1">
-        <v>201</v>
+        <v>356</v>
       </c>
       <c r="H35" s="1">
-        <v>301</v>
+        <v>447</v>
       </c>
       <c r="I35" s="1">
-        <v>639</v>
+        <v>533</v>
       </c>
       <c r="J35" s="1">
-        <v>495</v>
+        <v>374</v>
       </c>
       <c r="K35" s="1">
-        <v>350</v>
+        <v>775</v>
       </c>
       <c r="L35" s="1">
-        <v>1088</v>
+        <v>1130</v>
       </c>
       <c r="M35" s="1">
-        <v>1314</v>
+        <v>1437</v>
       </c>
       <c r="N35" s="1">
-        <v>1358</v>
+        <v>1564</v>
       </c>
       <c r="O35" s="1">
-        <v>1291</v>
+        <v>1226</v>
       </c>
       <c r="P35" s="1">
-        <v>1604</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C36" s="1">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E36" s="1">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="F36" s="1">
-        <v>237</v>
+        <v>283</v>
       </c>
       <c r="G36" s="1">
-        <v>231</v>
+        <v>329</v>
       </c>
       <c r="H36" s="1">
-        <v>414</v>
+        <v>187</v>
       </c>
       <c r="I36" s="1">
-        <v>483</v>
+        <v>676</v>
       </c>
       <c r="J36" s="1">
-        <v>817</v>
+        <v>274</v>
       </c>
       <c r="K36" s="1">
-        <v>664</v>
+        <v>647</v>
       </c>
       <c r="L36" s="1">
-        <v>1157</v>
+        <v>868</v>
       </c>
       <c r="M36" s="1">
-        <v>1378</v>
+        <v>1552</v>
       </c>
       <c r="N36" s="1">
-        <v>1431</v>
+        <v>1051</v>
       </c>
       <c r="O36" s="1">
-        <v>1315</v>
+        <v>1242</v>
       </c>
       <c r="P36" s="1">
-        <v>1648</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C37" s="1">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D37" s="1">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E37" s="1">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="F37" s="1">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="G37" s="1">
-        <v>322</v>
+        <v>201</v>
       </c>
       <c r="H37" s="1">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="I37" s="1">
-        <v>536</v>
+        <v>639</v>
       </c>
       <c r="J37" s="1">
-        <v>778</v>
+        <v>495</v>
       </c>
       <c r="K37" s="1">
-        <v>815</v>
+        <v>350</v>
       </c>
       <c r="L37" s="1">
-        <v>846</v>
+        <v>1088</v>
       </c>
       <c r="M37" s="1">
-        <v>1001</v>
+        <v>1314</v>
       </c>
       <c r="N37" s="1">
-        <v>1346</v>
+        <v>1358</v>
       </c>
       <c r="O37" s="1">
-        <v>1176</v>
+        <v>1291</v>
       </c>
       <c r="P37" s="1">
-        <v>2122</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C38" s="1">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D38" s="1">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E38" s="1">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="F38" s="1">
-        <v>136</v>
+        <v>237</v>
       </c>
       <c r="G38" s="1">
-        <v>169</v>
+        <v>231</v>
       </c>
       <c r="H38" s="1">
-        <v>497</v>
+        <v>414</v>
       </c>
       <c r="I38" s="1">
-        <v>667</v>
+        <v>483</v>
       </c>
       <c r="J38" s="1">
-        <v>564</v>
+        <v>817</v>
       </c>
       <c r="K38" s="1">
-        <v>810</v>
+        <v>664</v>
       </c>
       <c r="L38" s="1">
-        <v>881</v>
+        <v>1157</v>
       </c>
       <c r="M38" s="1">
-        <v>1263</v>
+        <v>1378</v>
       </c>
       <c r="N38" s="1">
-        <v>1437</v>
+        <v>1431</v>
       </c>
       <c r="O38" s="1">
-        <v>1417</v>
+        <v>1315</v>
       </c>
       <c r="P38" s="1">
-        <v>1900</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C39" s="1">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D39" s="1">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E39" s="1">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="F39" s="1">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="G39" s="1">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="H39" s="1">
-        <v>285</v>
+        <v>313</v>
       </c>
       <c r="I39" s="1">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="J39" s="1">
-        <v>346</v>
+        <v>778</v>
       </c>
       <c r="K39" s="1">
-        <v>415</v>
+        <v>815</v>
       </c>
       <c r="L39" s="1">
-        <v>1031</v>
+        <v>846</v>
       </c>
       <c r="M39" s="1">
-        <v>1675</v>
+        <v>1001</v>
       </c>
       <c r="N39" s="1">
-        <v>1253</v>
+        <v>1346</v>
       </c>
       <c r="O39" s="1">
-        <v>1373</v>
+        <v>1176</v>
       </c>
       <c r="P39" s="1">
-        <v>2425</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C40" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D40" s="1">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="E40" s="1">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F40" s="1">
-        <v>323</v>
+        <v>136</v>
       </c>
       <c r="G40" s="1">
-        <v>382</v>
+        <v>169</v>
       </c>
       <c r="H40" s="1">
-        <v>306</v>
+        <v>497</v>
       </c>
       <c r="I40" s="1">
-        <v>347</v>
+        <v>667</v>
       </c>
       <c r="J40" s="1">
-        <v>638</v>
+        <v>564</v>
       </c>
       <c r="K40" s="1">
-        <v>399</v>
+        <v>810</v>
       </c>
       <c r="L40" s="1">
-        <v>1386</v>
+        <v>881</v>
       </c>
       <c r="M40" s="1">
-        <v>1386</v>
+        <v>1263</v>
       </c>
       <c r="N40" s="1">
-        <v>1363</v>
+        <v>1437</v>
       </c>
       <c r="O40" s="1">
-        <v>1262</v>
+        <v>1417</v>
       </c>
       <c r="P40" s="1">
-        <v>2078</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C41" s="1">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D41" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E41" s="1">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="F41" s="1">
-        <v>237</v>
+        <v>158</v>
       </c>
       <c r="G41" s="1">
-        <v>317</v>
+        <v>335</v>
       </c>
       <c r="H41" s="1">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="I41" s="1">
-        <v>634</v>
+        <v>542</v>
       </c>
       <c r="J41" s="1">
-        <v>878</v>
+        <v>346</v>
       </c>
       <c r="K41" s="1">
-        <v>746</v>
+        <v>415</v>
       </c>
       <c r="L41" s="1">
-        <v>1116</v>
+        <v>1031</v>
       </c>
       <c r="M41" s="1">
-        <v>1519</v>
+        <v>1675</v>
       </c>
       <c r="N41" s="1">
-        <v>988</v>
+        <v>1253</v>
       </c>
       <c r="O41" s="1">
-        <v>1228</v>
+        <v>1373</v>
       </c>
       <c r="P41" s="1">
-        <v>1885</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C42" s="1">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D42" s="1">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="E42" s="1">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F42" s="1">
-        <v>230</v>
+        <v>323</v>
       </c>
       <c r="G42" s="1">
-        <v>518</v>
+        <v>382</v>
       </c>
       <c r="H42" s="1">
-        <v>214</v>
+        <v>306</v>
       </c>
       <c r="I42" s="1">
-        <v>656</v>
+        <v>347</v>
       </c>
       <c r="J42" s="1">
-        <v>551</v>
+        <v>638</v>
       </c>
       <c r="K42" s="1">
-        <v>424</v>
+        <v>399</v>
       </c>
       <c r="L42" s="1">
-        <v>1024</v>
+        <v>1386</v>
       </c>
       <c r="M42" s="1">
-        <v>1409</v>
+        <v>1386</v>
       </c>
       <c r="N42" s="1">
-        <v>1414</v>
+        <v>1363</v>
       </c>
       <c r="O42" s="1">
-        <v>1363</v>
+        <v>1262</v>
       </c>
       <c r="P42" s="1">
-        <v>1915</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C43" s="1">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D43" s="1">
         <v>77</v>
       </c>
       <c r="E43" s="1">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F43" s="1">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G43" s="1">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="H43" s="1">
-        <v>269</v>
+        <v>302</v>
       </c>
       <c r="I43" s="1">
-        <v>494</v>
+        <v>634</v>
       </c>
       <c r="J43" s="1">
-        <v>630</v>
+        <v>878</v>
       </c>
       <c r="K43" s="1">
-        <v>892</v>
+        <v>746</v>
       </c>
       <c r="L43" s="1">
-        <v>965</v>
+        <v>1116</v>
       </c>
       <c r="M43" s="1">
-        <v>1582</v>
+        <v>1519</v>
       </c>
       <c r="N43" s="1">
-        <v>1106</v>
+        <v>988</v>
       </c>
       <c r="O43" s="1">
-        <v>1291</v>
+        <v>1228</v>
       </c>
       <c r="P43" s="1">
-        <v>1997</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C44" s="1">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D44" s="1">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="E44" s="1">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F44" s="1">
-        <v>192</v>
+        <v>230</v>
       </c>
       <c r="G44" s="1">
-        <v>336</v>
+        <v>518</v>
       </c>
       <c r="H44" s="1">
-        <v>407</v>
+        <v>214</v>
       </c>
       <c r="I44" s="1">
-        <v>614</v>
+        <v>656</v>
       </c>
       <c r="J44" s="1">
-        <v>760</v>
+        <v>551</v>
       </c>
       <c r="K44" s="1">
-        <v>872</v>
+        <v>424</v>
       </c>
       <c r="L44" s="1">
-        <v>827</v>
+        <v>1024</v>
       </c>
       <c r="M44" s="1">
-        <v>1439</v>
+        <v>1409</v>
       </c>
       <c r="N44" s="1">
-        <v>989</v>
+        <v>1414</v>
       </c>
       <c r="O44" s="1">
-        <v>1121</v>
+        <v>1363</v>
       </c>
       <c r="P44" s="1">
-        <v>1976</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C45" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D45" s="1">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E45" s="1">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F45" s="1">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="G45" s="1">
-        <v>204</v>
+        <v>340</v>
       </c>
       <c r="H45" s="1">
-        <v>202</v>
+        <v>269</v>
       </c>
       <c r="I45" s="1">
-        <v>669</v>
+        <v>494</v>
       </c>
       <c r="J45" s="1">
-        <v>754</v>
+        <v>630</v>
       </c>
       <c r="K45" s="1">
-        <v>769</v>
+        <v>892</v>
       </c>
       <c r="L45" s="1">
-        <v>413</v>
+        <v>965</v>
       </c>
       <c r="M45" s="1">
-        <v>1298</v>
+        <v>1582</v>
       </c>
       <c r="N45" s="1">
-        <v>991</v>
+        <v>1106</v>
       </c>
       <c r="O45" s="1">
-        <v>1230</v>
+        <v>1291</v>
       </c>
       <c r="P45" s="1">
-        <v>1877</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C46" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D46" s="1">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E46" s="1">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="F46" s="1">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="G46" s="1">
-        <v>236</v>
+        <v>336</v>
       </c>
       <c r="H46" s="1">
-        <v>226</v>
+        <v>407</v>
       </c>
       <c r="I46" s="1">
-        <v>660</v>
+        <v>614</v>
       </c>
       <c r="J46" s="1">
-        <v>677</v>
+        <v>760</v>
       </c>
       <c r="K46" s="1">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="L46" s="1">
-        <v>929</v>
+        <v>827</v>
       </c>
       <c r="M46" s="1">
-        <v>1613</v>
+        <v>1439</v>
       </c>
       <c r="N46" s="1">
-        <v>1136</v>
+        <v>989</v>
       </c>
       <c r="O46" s="1">
-        <v>1308</v>
+        <v>1121</v>
       </c>
       <c r="P46" s="1">
-        <v>2021</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C47" s="1">
         <v>40</v>
       </c>
       <c r="D47" s="1">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E47" s="1">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="F47" s="1">
-        <v>240</v>
+        <v>273</v>
       </c>
       <c r="G47" s="1">
-        <v>153</v>
+        <v>204</v>
       </c>
       <c r="H47" s="1">
-        <v>429</v>
+        <v>202</v>
       </c>
       <c r="I47" s="1">
-        <v>692</v>
+        <v>669</v>
       </c>
       <c r="J47" s="1">
-        <v>449</v>
+        <v>754</v>
       </c>
       <c r="K47" s="1">
-        <v>448</v>
+        <v>769</v>
       </c>
       <c r="L47" s="1">
-        <v>735</v>
+        <v>413</v>
       </c>
       <c r="M47" s="1">
-        <v>1244</v>
+        <v>1298</v>
       </c>
       <c r="N47" s="1">
-        <v>1090</v>
+        <v>991</v>
       </c>
       <c r="O47" s="1">
-        <v>1297</v>
+        <v>1230</v>
       </c>
       <c r="P47" s="1">
-        <v>1871</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C48" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D48" s="1">
         <v>82</v>
       </c>
       <c r="E48" s="1">
+        <v>106</v>
+      </c>
+      <c r="F48" s="1">
+        <v>183</v>
+      </c>
+      <c r="G48" s="1">
+        <v>236</v>
+      </c>
+      <c r="H48" s="1">
+        <v>226</v>
+      </c>
+      <c r="I48" s="1">
+        <v>660</v>
+      </c>
+      <c r="J48" s="1">
+        <v>677</v>
+      </c>
+      <c r="K48" s="1">
+        <v>870</v>
+      </c>
+      <c r="L48" s="1">
+        <v>929</v>
+      </c>
+      <c r="M48" s="1">
+        <v>1613</v>
+      </c>
+      <c r="N48" s="1">
+        <v>1136</v>
+      </c>
+      <c r="O48" s="1">
+        <v>1308</v>
+      </c>
+      <c r="P48" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>34</v>
+      </c>
+      <c r="C49" s="1">
+        <v>40</v>
+      </c>
+      <c r="D49" s="1">
+        <v>76</v>
+      </c>
+      <c r="E49" s="1">
         <v>149</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F49" s="1">
+        <v>240</v>
+      </c>
+      <c r="G49" s="1">
+        <v>153</v>
+      </c>
+      <c r="H49" s="1">
+        <v>429</v>
+      </c>
+      <c r="I49" s="1">
+        <v>692</v>
+      </c>
+      <c r="J49" s="1">
+        <v>449</v>
+      </c>
+      <c r="K49" s="1">
+        <v>448</v>
+      </c>
+      <c r="L49" s="1">
+        <v>735</v>
+      </c>
+      <c r="M49" s="1">
+        <v>1244</v>
+      </c>
+      <c r="N49" s="1">
+        <v>1090</v>
+      </c>
+      <c r="O49" s="1">
+        <v>1297</v>
+      </c>
+      <c r="P49" s="1">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
+        <v>29</v>
+      </c>
+      <c r="C50" s="1">
+        <v>39</v>
+      </c>
+      <c r="D50" s="1">
+        <v>82</v>
+      </c>
+      <c r="E50" s="1">
+        <v>149</v>
+      </c>
+      <c r="F50" s="1">
         <v>233</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G50" s="1">
         <v>309</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H50" s="1">
         <v>311</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I50" s="1">
         <v>628</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J50" s="1">
         <v>736</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K50" s="1">
         <v>878</v>
       </c>
-      <c r="L48" s="1">
+      <c r="L50" s="1">
         <v>559</v>
       </c>
-      <c r="M48" s="1">
+      <c r="M50" s="1">
         <v>1762</v>
       </c>
-      <c r="N48" s="1">
+      <c r="N50" s="1">
         <v>1090</v>
       </c>
-      <c r="O48" s="1">
+      <c r="O50" s="1">
         <v>1339</v>
       </c>
-      <c r="P48" s="1">
+      <c r="P50" s="1">
         <v>1989</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="1">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
         <v>37</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C51" s="1">
         <v>34</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D51" s="1">
         <v>93</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E51" s="1">
         <v>122</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F51" s="1">
         <v>209</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G51" s="1">
         <v>312</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H51" s="1">
         <v>338</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I51" s="1">
         <v>591</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J51" s="1">
         <v>715</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K51" s="1">
         <v>911</v>
       </c>
-      <c r="L49" s="1">
+      <c r="L51" s="1">
         <v>833</v>
       </c>
-      <c r="M49" s="1">
+      <c r="M51" s="1">
         <v>1626</v>
       </c>
-      <c r="N49" s="1">
+      <c r="N51" s="1">
         <v>1145</v>
       </c>
-      <c r="O49" s="1">
+      <c r="O51" s="1">
         <v>1143</v>
       </c>
-      <c r="P49" s="1">
+      <c r="P51" s="1">
         <v>1727</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="1">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
         <v>27</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C52" s="1">
         <v>37</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D52" s="1">
         <v>89</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E52" s="1">
         <v>102</v>
-      </c>
-      <c r="F50" s="1">
-        <v>196</v>
-      </c>
-      <c r="G50" s="1">
-        <v>341</v>
-      </c>
-      <c r="H50" s="1">
-        <v>240</v>
-      </c>
-      <c r="I50" s="1">
-        <v>339</v>
-      </c>
-      <c r="J50" s="1">
-        <v>682</v>
-      </c>
-      <c r="K50" s="1">
-        <v>912</v>
-      </c>
-      <c r="L50" s="1">
-        <v>751</v>
-      </c>
-      <c r="M50" s="1">
-        <v>1787</v>
-      </c>
-      <c r="N50" s="1">
-        <v>1095</v>
-      </c>
-      <c r="O50" s="1">
-        <v>1260</v>
-      </c>
-      <c r="P50" s="1">
-        <v>1830</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="1">
-        <v>30</v>
-      </c>
-      <c r="C51" s="1">
-        <v>32</v>
-      </c>
-      <c r="D51" s="1">
-        <v>71</v>
-      </c>
-      <c r="E51" s="1">
-        <v>125</v>
-      </c>
-      <c r="F51" s="1">
-        <v>171</v>
-      </c>
-      <c r="G51" s="1">
-        <v>361</v>
-      </c>
-      <c r="H51" s="1">
-        <v>466</v>
-      </c>
-      <c r="I51" s="1">
-        <v>579</v>
-      </c>
-      <c r="J51" s="1">
-        <v>647</v>
-      </c>
-      <c r="K51" s="1">
-        <v>366</v>
-      </c>
-      <c r="L51" s="1">
-        <v>664</v>
-      </c>
-      <c r="M51" s="1">
-        <v>1668</v>
-      </c>
-      <c r="N51" s="1">
-        <v>1127</v>
-      </c>
-      <c r="O51" s="1">
-        <v>1312</v>
-      </c>
-      <c r="P51" s="1">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B52" s="1">
-        <v>29</v>
-      </c>
-      <c r="C52" s="1">
-        <v>34</v>
-      </c>
-      <c r="D52" s="1">
-        <v>83</v>
-      </c>
-      <c r="E52" s="1">
-        <v>168</v>
       </c>
       <c r="F52" s="1">
         <v>196</v>
       </c>
       <c r="G52" s="1">
-        <v>166</v>
+        <v>341</v>
       </c>
       <c r="H52" s="1">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I52" s="1">
-        <v>668</v>
+        <v>339</v>
       </c>
       <c r="J52" s="1">
-        <v>755</v>
+        <v>682</v>
       </c>
       <c r="K52" s="1">
-        <v>354</v>
+        <v>912</v>
       </c>
       <c r="L52" s="1">
-        <v>939</v>
+        <v>751</v>
       </c>
       <c r="M52" s="1">
-        <v>1690</v>
+        <v>1787</v>
       </c>
       <c r="N52" s="1">
-        <v>1048</v>
+        <v>1095</v>
       </c>
       <c r="O52" s="1">
-        <v>1275</v>
+        <v>1260</v>
       </c>
       <c r="P52" s="1">
-        <v>2074</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C53" s="1">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D53" s="1">
         <v>71</v>
       </c>
       <c r="E53" s="1">
+        <v>125</v>
+      </c>
+      <c r="F53" s="1">
+        <v>171</v>
+      </c>
+      <c r="G53" s="1">
+        <v>361</v>
+      </c>
+      <c r="H53" s="1">
+        <v>466</v>
+      </c>
+      <c r="I53" s="1">
+        <v>579</v>
+      </c>
+      <c r="J53" s="1">
+        <v>647</v>
+      </c>
+      <c r="K53" s="1">
+        <v>366</v>
+      </c>
+      <c r="L53" s="1">
+        <v>664</v>
+      </c>
+      <c r="M53" s="1">
+        <v>1668</v>
+      </c>
+      <c r="N53" s="1">
+        <v>1127</v>
+      </c>
+      <c r="O53" s="1">
+        <v>1312</v>
+      </c>
+      <c r="P53" s="1">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>29</v>
+      </c>
+      <c r="C54" s="1">
+        <v>34</v>
+      </c>
+      <c r="D54" s="1">
+        <v>83</v>
+      </c>
+      <c r="E54" s="1">
+        <v>168</v>
+      </c>
+      <c r="F54" s="1">
+        <v>196</v>
+      </c>
+      <c r="G54" s="1">
+        <v>166</v>
+      </c>
+      <c r="H54" s="1">
+        <v>233</v>
+      </c>
+      <c r="I54" s="1">
+        <v>668</v>
+      </c>
+      <c r="J54" s="1">
+        <v>755</v>
+      </c>
+      <c r="K54" s="1">
+        <v>354</v>
+      </c>
+      <c r="L54" s="1">
+        <v>939</v>
+      </c>
+      <c r="M54" s="1">
+        <v>1690</v>
+      </c>
+      <c r="N54" s="1">
+        <v>1048</v>
+      </c>
+      <c r="O54" s="1">
+        <v>1275</v>
+      </c>
+      <c r="P54" s="1">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>37</v>
+      </c>
+      <c r="C55" s="1">
+        <v>47</v>
+      </c>
+      <c r="D55" s="1">
+        <v>71</v>
+      </c>
+      <c r="E55" s="1">
         <v>159</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F55" s="1">
         <v>180</v>
       </c>
-      <c r="G53" s="1">
+      <c r="G55" s="1">
         <v>303</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H55" s="1">
         <v>213</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I55" s="1">
         <v>578</v>
       </c>
-      <c r="J53" s="1">
+      <c r="J55" s="1">
         <v>761</v>
       </c>
-      <c r="K53" s="1">
+      <c r="K55" s="1">
         <v>381</v>
       </c>
-      <c r="L53" s="1">
+      <c r="L55" s="1">
         <v>457</v>
       </c>
-      <c r="M53" s="1">
+      <c r="M55" s="1">
         <v>1669</v>
       </c>
-      <c r="N53" s="1">
+      <c r="N55" s="1">
         <v>1068</v>
       </c>
-      <c r="O53" s="1">
+      <c r="O55" s="1">
         <v>1433</v>
       </c>
-      <c r="P53" s="1">
+      <c r="P55" s="1">
         <v>2373</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="1">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
         <v>25</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C56" s="1">
         <v>59</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D56" s="1">
         <v>85</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E56" s="1">
         <v>130</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F56" s="1">
         <v>206</v>
       </c>
-      <c r="G54" s="1">
+      <c r="G56" s="1">
         <v>379</v>
       </c>
-      <c r="H54" s="1">
+      <c r="H56" s="1">
         <v>226</v>
       </c>
-      <c r="I54" s="1">
+      <c r="I56" s="1">
         <v>268</v>
       </c>
-      <c r="J54" s="1">
+      <c r="J56" s="1">
         <v>839</v>
       </c>
-      <c r="K54" s="1">
+      <c r="K56" s="1">
         <v>692</v>
       </c>
-      <c r="L54" s="1">
+      <c r="L56" s="1">
         <v>725</v>
       </c>
-      <c r="M54" s="1">
+      <c r="M56" s="1">
         <v>1734</v>
       </c>
-      <c r="N54" s="1">
+      <c r="N56" s="1">
         <v>1314</v>
       </c>
-      <c r="O54" s="1">
+      <c r="O56" s="1">
         <v>1352</v>
       </c>
-      <c r="P54" s="1">
+      <c r="P56" s="1">
         <v>1429</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="1">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
         <v>15</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C57" s="1">
         <v>41</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D57" s="1">
         <v>83</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E57" s="1">
         <v>105</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F57" s="1">
         <v>159</v>
       </c>
-      <c r="G55" s="1">
+      <c r="G57" s="1">
         <v>203</v>
       </c>
-      <c r="H55" s="1">
+      <c r="H57" s="1">
         <v>299</v>
       </c>
-      <c r="I55" s="1">
+      <c r="I57" s="1">
         <v>271</v>
       </c>
-      <c r="J55" s="1">
+      <c r="J57" s="1">
         <v>717</v>
       </c>
-      <c r="K55" s="1">
+      <c r="K57" s="1">
         <v>863</v>
       </c>
-      <c r="L55" s="1">
+      <c r="L57" s="1">
         <v>905</v>
       </c>
-      <c r="M55" s="1">
+      <c r="M57" s="1">
         <v>1856</v>
       </c>
-      <c r="N55" s="1">
+      <c r="N57" s="1">
         <v>928</v>
       </c>
-      <c r="O55" s="1">
+      <c r="O57" s="1">
         <v>1306</v>
       </c>
-      <c r="P55" s="1">
+      <c r="P57" s="1">
         <v>2157</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B56" s="1">
-        <v>26</v>
-      </c>
-      <c r="C56" s="1">
-        <v>30</v>
-      </c>
-      <c r="D56" s="1">
-        <v>84</v>
-      </c>
-      <c r="E56" s="1">
-        <v>110</v>
-      </c>
-      <c r="F56" s="1">
-        <v>155</v>
-      </c>
-      <c r="G56" s="1">
-        <v>245</v>
-      </c>
-      <c r="H56" s="1">
-        <v>607</v>
-      </c>
-      <c r="I56" s="1">
-        <v>341</v>
-      </c>
-      <c r="J56" s="1">
-        <v>788</v>
-      </c>
-      <c r="K56" s="1">
-        <v>309</v>
-      </c>
-      <c r="L56" s="1">
-        <v>1013</v>
-      </c>
-      <c r="M56" s="1">
-        <v>1721</v>
-      </c>
-      <c r="N56" s="1">
-        <v>1433</v>
-      </c>
-      <c r="O56" s="1">
-        <v>917</v>
-      </c>
-      <c r="P56" s="1">
-        <v>2432</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B57" s="1">
-        <v>24</v>
-      </c>
-      <c r="C57" s="1">
-        <v>35</v>
-      </c>
-      <c r="D57" s="1">
-        <v>70</v>
-      </c>
-      <c r="E57" s="1">
-        <v>107</v>
-      </c>
-      <c r="F57" s="1">
-        <v>186</v>
-      </c>
-      <c r="G57" s="1">
-        <v>264</v>
-      </c>
-      <c r="H57" s="1">
-        <v>585</v>
-      </c>
-      <c r="I57" s="1">
-        <v>368</v>
-      </c>
-      <c r="J57" s="1">
-        <v>562</v>
-      </c>
-      <c r="K57" s="1">
-        <v>762</v>
-      </c>
-      <c r="L57" s="1">
-        <v>1078</v>
-      </c>
-      <c r="M57" s="1">
-        <v>1624</v>
-      </c>
-      <c r="N57" s="1">
-        <v>1134</v>
-      </c>
-      <c r="O57" s="1">
-        <v>1135</v>
-      </c>
-      <c r="P57" s="1">
-        <v>2363</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>26</v>
       </c>
       <c r="C58" s="1">
+        <v>30</v>
+      </c>
+      <c r="D58" s="1">
+        <v>84</v>
+      </c>
+      <c r="E58" s="1">
+        <v>110</v>
+      </c>
+      <c r="F58" s="1">
+        <v>155</v>
+      </c>
+      <c r="G58" s="1">
+        <v>245</v>
+      </c>
+      <c r="H58" s="1">
+        <v>607</v>
+      </c>
+      <c r="I58" s="1">
+        <v>341</v>
+      </c>
+      <c r="J58" s="1">
+        <v>788</v>
+      </c>
+      <c r="K58" s="1">
+        <v>309</v>
+      </c>
+      <c r="L58" s="1">
+        <v>1013</v>
+      </c>
+      <c r="M58" s="1">
+        <v>1721</v>
+      </c>
+      <c r="N58" s="1">
+        <v>1433</v>
+      </c>
+      <c r="O58" s="1">
+        <v>917</v>
+      </c>
+      <c r="P58" s="1">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>24</v>
+      </c>
+      <c r="C59" s="1">
+        <v>35</v>
+      </c>
+      <c r="D59" s="1">
+        <v>70</v>
+      </c>
+      <c r="E59" s="1">
+        <v>107</v>
+      </c>
+      <c r="F59" s="1">
+        <v>186</v>
+      </c>
+      <c r="G59" s="1">
+        <v>264</v>
+      </c>
+      <c r="H59" s="1">
+        <v>585</v>
+      </c>
+      <c r="I59" s="1">
+        <v>368</v>
+      </c>
+      <c r="J59" s="1">
+        <v>562</v>
+      </c>
+      <c r="K59" s="1">
+        <v>762</v>
+      </c>
+      <c r="L59" s="1">
+        <v>1078</v>
+      </c>
+      <c r="M59" s="1">
+        <v>1624</v>
+      </c>
+      <c r="N59" s="1">
+        <v>1134</v>
+      </c>
+      <c r="O59" s="1">
+        <v>1135</v>
+      </c>
+      <c r="P59" s="1">
+        <v>2363</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <v>26</v>
+      </c>
+      <c r="C60" s="1">
         <v>38</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D60" s="1">
         <v>71</v>
-      </c>
-      <c r="E58" s="1">
-        <v>113</v>
-      </c>
-      <c r="F58" s="1">
-        <v>272</v>
-      </c>
-      <c r="G58" s="1">
-        <v>285</v>
-      </c>
-      <c r="H58" s="1">
-        <v>502</v>
-      </c>
-      <c r="I58" s="1">
-        <v>275</v>
-      </c>
-      <c r="J58" s="1">
-        <v>611</v>
-      </c>
-      <c r="K58" s="1">
-        <v>619</v>
-      </c>
-      <c r="L58" s="1">
-        <v>806</v>
-      </c>
-      <c r="M58" s="1">
-        <v>1484</v>
-      </c>
-      <c r="N58" s="1">
-        <v>822</v>
-      </c>
-      <c r="O58" s="1">
-        <v>1408</v>
-      </c>
-      <c r="P58" s="1">
-        <v>2364</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B59" s="1">
-        <v>34</v>
-      </c>
-      <c r="C59" s="1">
-        <v>48</v>
-      </c>
-      <c r="D59" s="1">
-        <v>89</v>
-      </c>
-      <c r="E59" s="1">
-        <v>101</v>
-      </c>
-      <c r="F59" s="1">
-        <v>240</v>
-      </c>
-      <c r="G59" s="1">
-        <v>224</v>
-      </c>
-      <c r="H59" s="1">
-        <v>501</v>
-      </c>
-      <c r="I59" s="1">
-        <v>373</v>
-      </c>
-      <c r="J59" s="1">
-        <v>584</v>
-      </c>
-      <c r="K59" s="1">
-        <v>1202</v>
-      </c>
-      <c r="L59" s="1">
-        <v>1058</v>
-      </c>
-      <c r="M59" s="1">
-        <v>1370</v>
-      </c>
-      <c r="N59" s="1">
-        <v>1285</v>
-      </c>
-      <c r="O59" s="1">
-        <v>1273</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B60" s="1">
-        <v>37</v>
-      </c>
-      <c r="C60" s="1">
-        <v>29</v>
-      </c>
-      <c r="D60" s="1">
-        <v>80</v>
       </c>
       <c r="E60" s="1">
         <v>113</v>
       </c>
       <c r="F60" s="1">
+        <v>272</v>
+      </c>
+      <c r="G60" s="1">
+        <v>285</v>
+      </c>
+      <c r="H60" s="1">
+        <v>502</v>
+      </c>
+      <c r="I60" s="1">
+        <v>275</v>
+      </c>
+      <c r="J60" s="1">
+        <v>611</v>
+      </c>
+      <c r="K60" s="1">
+        <v>619</v>
+      </c>
+      <c r="L60" s="1">
+        <v>806</v>
+      </c>
+      <c r="M60" s="1">
+        <v>1484</v>
+      </c>
+      <c r="N60" s="1">
+        <v>822</v>
+      </c>
+      <c r="O60" s="1">
+        <v>1408</v>
+      </c>
+      <c r="P60" s="1">
+        <v>2364</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>34</v>
+      </c>
+      <c r="C61" s="1">
+        <v>48</v>
+      </c>
+      <c r="D61" s="1">
+        <v>89</v>
+      </c>
+      <c r="E61" s="1">
+        <v>101</v>
+      </c>
+      <c r="F61" s="1">
+        <v>240</v>
+      </c>
+      <c r="G61" s="1">
+        <v>224</v>
+      </c>
+      <c r="H61" s="1">
+        <v>501</v>
+      </c>
+      <c r="I61" s="1">
+        <v>373</v>
+      </c>
+      <c r="J61" s="1">
+        <v>584</v>
+      </c>
+      <c r="K61" s="1">
+        <v>1202</v>
+      </c>
+      <c r="L61" s="1">
+        <v>1058</v>
+      </c>
+      <c r="M61" s="1">
+        <v>1370</v>
+      </c>
+      <c r="N61" s="1">
+        <v>1285</v>
+      </c>
+      <c r="O61" s="1">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
+        <v>37</v>
+      </c>
+      <c r="C62" s="1">
+        <v>29</v>
+      </c>
+      <c r="D62" s="1">
+        <v>80</v>
+      </c>
+      <c r="E62" s="1">
+        <v>113</v>
+      </c>
+      <c r="F62" s="1">
         <v>152</v>
       </c>
-      <c r="G60" s="1">
+      <c r="G62" s="1">
         <v>356</v>
       </c>
-      <c r="H60" s="1">
+      <c r="H62" s="1">
         <v>523</v>
       </c>
-      <c r="I60" s="1">
+      <c r="I62" s="1">
         <v>617</v>
       </c>
-      <c r="J60" s="1">
+      <c r="J62" s="1">
         <v>734</v>
       </c>
-      <c r="K60" s="1">
+      <c r="K62" s="1">
         <v>1372</v>
       </c>
-      <c r="L60" s="1">
+      <c r="L62" s="1">
         <v>1099</v>
       </c>
-      <c r="M60" s="1">
+      <c r="M62" s="1">
         <v>1490</v>
       </c>
-      <c r="N60" s="1">
+      <c r="N62" s="1">
         <v>1086</v>
       </c>
-      <c r="O60" s="1">
+      <c r="O62" s="1">
         <v>1404</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="1">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
         <v>25</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C63" s="1">
         <v>33</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D63" s="1">
         <v>79</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E63" s="1">
         <v>120</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F63" s="1">
         <v>229</v>
       </c>
-      <c r="G61" s="1">
+      <c r="G63" s="1">
         <v>234</v>
       </c>
-      <c r="H61" s="1">
+      <c r="H63" s="1">
         <v>423</v>
       </c>
-      <c r="I61" s="1">
+      <c r="I63" s="1">
         <v>471</v>
       </c>
-      <c r="J61" s="1">
+      <c r="J63" s="1">
         <v>764</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K63" s="1">
         <v>1161</v>
       </c>
-      <c r="L61" s="1">
+      <c r="L63" s="1">
         <v>758</v>
       </c>
-      <c r="M61" s="1">
+      <c r="M63" s="1">
         <v>1347</v>
       </c>
-      <c r="N61" s="1">
+      <c r="N63" s="1">
         <v>1163</v>
       </c>
-      <c r="O61" s="1">
+      <c r="O63" s="1">
         <v>1366</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="K66" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L64" s="2" t="s">
+      <c r="L66" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M64" s="2" t="s">
+      <c r="M66" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N64" s="2" t="s">
+      <c r="N66" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O64" s="2" t="s">
+      <c r="O66" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P64" s="2" t="s">
+      <c r="P66" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B65" s="1">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
         <v>47</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C67" s="1">
         <v>43</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D67" s="1">
         <v>139</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E67" s="1">
         <v>146</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F67" s="1">
         <v>293</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G67" s="1">
         <v>509</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H67" s="1">
         <v>600</v>
       </c>
-      <c r="I65" s="1">
+      <c r="I67" s="1">
         <v>836</v>
       </c>
-      <c r="J65" s="1">
+      <c r="J67" s="1">
         <v>785</v>
       </c>
-      <c r="K65" s="1">
+      <c r="K67" s="1">
         <v>1001</v>
       </c>
-      <c r="L65" s="1">
+      <c r="L67" s="1">
         <v>1153</v>
       </c>
-      <c r="M65" s="1">
+      <c r="M67" s="1">
         <v>1331</v>
       </c>
-      <c r="N65" s="1">
+      <c r="N67" s="1">
         <v>2070</v>
       </c>
-      <c r="O65" s="1">
+      <c r="O67" s="1">
         <v>1561</v>
       </c>
-      <c r="P65" s="1">
+      <c r="P67" s="1">
         <v>1730</v>
       </c>
     </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B66" s="1">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
         <v>18</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C68" s="1">
         <v>34</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D68" s="1">
         <v>258</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E68" s="1">
         <v>212</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F68" s="1">
         <v>231</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G68" s="1">
         <v>482</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H68" s="1">
         <v>725</v>
       </c>
-      <c r="I66" s="1">
+      <c r="I68" s="1">
         <v>863</v>
       </c>
-      <c r="J66" s="1">
+      <c r="J68" s="1">
         <v>999</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K68" s="1">
         <v>1109</v>
       </c>
-      <c r="L66" s="1">
+      <c r="L68" s="1">
         <v>1541</v>
       </c>
-      <c r="M66" s="1">
+      <c r="M68" s="1">
         <v>1435</v>
       </c>
-      <c r="N66" s="1">
+      <c r="N68" s="1">
         <v>1892</v>
       </c>
-      <c r="O66" s="1">
+      <c r="O68" s="1">
         <v>1345</v>
       </c>
-      <c r="P66" s="1">
+      <c r="P68" s="1">
         <v>2526</v>
       </c>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B67" s="1">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
         <v>35</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C69" s="1">
         <v>52</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D69" s="1">
         <v>87</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E69" s="1">
         <v>126</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F69" s="1">
         <v>176</v>
-      </c>
-      <c r="G67" s="1">
-        <v>462</v>
-      </c>
-      <c r="H67" s="1">
-        <v>605</v>
-      </c>
-      <c r="I67" s="1">
-        <v>783</v>
-      </c>
-      <c r="J67" s="1">
-        <v>1037</v>
-      </c>
-      <c r="K67" s="1">
-        <v>1090</v>
-      </c>
-      <c r="L67" s="1">
-        <v>1207</v>
-      </c>
-      <c r="M67" s="1">
-        <v>1508</v>
-      </c>
-      <c r="N67" s="1">
-        <v>1723</v>
-      </c>
-      <c r="O67" s="1">
-        <v>1407</v>
-      </c>
-      <c r="P67" s="1">
-        <v>2160</v>
-      </c>
-    </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B68" s="1">
-        <v>46</v>
-      </c>
-      <c r="C68" s="1">
-        <v>56</v>
-      </c>
-      <c r="D68" s="1">
-        <v>95</v>
-      </c>
-      <c r="E68" s="1">
-        <v>111</v>
-      </c>
-      <c r="F68" s="1">
-        <v>347</v>
-      </c>
-      <c r="G68" s="1">
-        <v>496</v>
-      </c>
-      <c r="H68" s="1">
-        <v>659</v>
-      </c>
-      <c r="I68" s="1">
-        <v>892</v>
-      </c>
-      <c r="J68" s="1">
-        <v>920</v>
-      </c>
-      <c r="K68" s="1">
-        <v>1063</v>
-      </c>
-      <c r="L68" s="1">
-        <v>1259</v>
-      </c>
-      <c r="M68" s="1">
-        <v>1276</v>
-      </c>
-      <c r="N68" s="1">
-        <v>1456</v>
-      </c>
-      <c r="O68" s="1">
-        <v>1440</v>
-      </c>
-      <c r="P68" s="1">
-        <v>1867</v>
-      </c>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B69" s="1">
-        <v>40</v>
-      </c>
-      <c r="C69" s="1">
-        <v>45</v>
-      </c>
-      <c r="D69" s="1">
-        <v>195</v>
-      </c>
-      <c r="E69" s="1">
-        <v>168</v>
-      </c>
-      <c r="F69" s="1">
-        <v>356</v>
       </c>
       <c r="G69" s="1">
         <v>462</v>
       </c>
       <c r="H69" s="1">
+        <v>605</v>
+      </c>
+      <c r="I69" s="1">
+        <v>783</v>
+      </c>
+      <c r="J69" s="1">
+        <v>1037</v>
+      </c>
+      <c r="K69" s="1">
+        <v>1090</v>
+      </c>
+      <c r="L69" s="1">
+        <v>1207</v>
+      </c>
+      <c r="M69" s="1">
+        <v>1508</v>
+      </c>
+      <c r="N69" s="1">
+        <v>1723</v>
+      </c>
+      <c r="O69" s="1">
+        <v>1407</v>
+      </c>
+      <c r="P69" s="1">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>46</v>
+      </c>
+      <c r="C70" s="1">
+        <v>56</v>
+      </c>
+      <c r="D70" s="1">
+        <v>95</v>
+      </c>
+      <c r="E70" s="1">
+        <v>111</v>
+      </c>
+      <c r="F70" s="1">
+        <v>347</v>
+      </c>
+      <c r="G70" s="1">
+        <v>496</v>
+      </c>
+      <c r="H70" s="1">
+        <v>659</v>
+      </c>
+      <c r="I70" s="1">
+        <v>892</v>
+      </c>
+      <c r="J70" s="1">
+        <v>920</v>
+      </c>
+      <c r="K70" s="1">
+        <v>1063</v>
+      </c>
+      <c r="L70" s="1">
+        <v>1259</v>
+      </c>
+      <c r="M70" s="1">
+        <v>1276</v>
+      </c>
+      <c r="N70" s="1">
+        <v>1456</v>
+      </c>
+      <c r="O70" s="1">
+        <v>1440</v>
+      </c>
+      <c r="P70" s="1">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
+        <v>40</v>
+      </c>
+      <c r="C71" s="1">
+        <v>45</v>
+      </c>
+      <c r="D71" s="1">
+        <v>195</v>
+      </c>
+      <c r="E71" s="1">
+        <v>168</v>
+      </c>
+      <c r="F71" s="1">
+        <v>356</v>
+      </c>
+      <c r="G71" s="1">
+        <v>462</v>
+      </c>
+      <c r="H71" s="1">
         <v>628</v>
       </c>
-      <c r="I69" s="1">
+      <c r="I71" s="1">
         <v>780</v>
       </c>
-      <c r="J69" s="1">
+      <c r="J71" s="1">
         <v>965</v>
       </c>
-      <c r="K69" s="1">
+      <c r="K71" s="1">
         <v>1058</v>
       </c>
-      <c r="L69" s="1">
+      <c r="L71" s="1">
         <v>1209</v>
       </c>
-      <c r="M69" s="1">
+      <c r="M71" s="1">
         <v>1638</v>
       </c>
-      <c r="N69" s="1">
+      <c r="N71" s="1">
         <v>1477</v>
       </c>
-      <c r="O69" s="1">
+      <c r="O71" s="1">
         <v>1418</v>
       </c>
-      <c r="P69" s="1">
+      <c r="P71" s="1">
         <v>1781</v>
       </c>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B70" s="1">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
         <v>45</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C72" s="1">
         <v>52</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D72" s="1">
         <v>135</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E72" s="1">
         <v>134</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F72" s="1">
         <v>337</v>
-      </c>
-      <c r="G70" s="1">
-        <v>503</v>
-      </c>
-      <c r="H70" s="1">
-        <v>674</v>
-      </c>
-      <c r="I70" s="1">
-        <v>851</v>
-      </c>
-      <c r="J70" s="1">
-        <v>779</v>
-      </c>
-      <c r="K70" s="1">
-        <v>1226</v>
-      </c>
-      <c r="L70" s="1">
-        <v>1079</v>
-      </c>
-      <c r="M70" s="1">
-        <v>1515</v>
-      </c>
-      <c r="N70" s="1">
-        <v>1545</v>
-      </c>
-      <c r="O70" s="1">
-        <v>1377</v>
-      </c>
-      <c r="P70" s="1">
-        <v>1701</v>
-      </c>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B71" s="1">
-        <v>43</v>
-      </c>
-      <c r="C71" s="1">
-        <v>48</v>
-      </c>
-      <c r="D71" s="1">
-        <v>91</v>
-      </c>
-      <c r="E71" s="1">
-        <v>149</v>
-      </c>
-      <c r="F71" s="1">
-        <v>352</v>
-      </c>
-      <c r="G71" s="1">
-        <v>525</v>
-      </c>
-      <c r="H71" s="1">
-        <v>631</v>
-      </c>
-      <c r="I71" s="1">
-        <v>790</v>
-      </c>
-      <c r="J71" s="1">
-        <v>789</v>
-      </c>
-      <c r="K71" s="1">
-        <v>1186</v>
-      </c>
-      <c r="L71" s="1">
-        <v>1260</v>
-      </c>
-      <c r="M71" s="1">
-        <v>1624</v>
-      </c>
-      <c r="N71" s="1">
-        <v>1516</v>
-      </c>
-      <c r="O71" s="1">
-        <v>1393</v>
-      </c>
-      <c r="P71" s="1">
-        <v>2239</v>
-      </c>
-    </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B72" s="1">
-        <v>37</v>
-      </c>
-      <c r="C72" s="1">
-        <v>57</v>
-      </c>
-      <c r="D72" s="1">
-        <v>195</v>
-      </c>
-      <c r="E72" s="1">
-        <v>129</v>
-      </c>
-      <c r="F72" s="1">
-        <v>346</v>
       </c>
       <c r="G72" s="1">
         <v>503</v>
       </c>
       <c r="H72" s="1">
-        <v>650</v>
+        <v>674</v>
       </c>
       <c r="I72" s="1">
-        <v>812</v>
+        <v>851</v>
       </c>
       <c r="J72" s="1">
-        <v>695</v>
+        <v>779</v>
       </c>
       <c r="K72" s="1">
-        <v>1053</v>
+        <v>1226</v>
       </c>
       <c r="L72" s="1">
-        <v>1085</v>
+        <v>1079</v>
       </c>
       <c r="M72" s="1">
-        <v>1584</v>
+        <v>1515</v>
       </c>
       <c r="N72" s="1">
-        <v>1613</v>
+        <v>1545</v>
       </c>
       <c r="O72" s="1">
-        <v>1495</v>
+        <v>1377</v>
       </c>
       <c r="P72" s="1">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B73" s="1">
         <v>43</v>
       </c>
       <c r="C73" s="1">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D73" s="1">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E73" s="1">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="F73" s="1">
-        <v>287</v>
+        <v>352</v>
       </c>
       <c r="G73" s="1">
-        <v>515</v>
+        <v>525</v>
       </c>
       <c r="H73" s="1">
-        <v>681</v>
+        <v>631</v>
       </c>
       <c r="I73" s="1">
-        <v>806</v>
+        <v>790</v>
       </c>
       <c r="J73" s="1">
-        <v>828</v>
+        <v>789</v>
       </c>
       <c r="K73" s="1">
-        <v>1025</v>
+        <v>1186</v>
       </c>
       <c r="L73" s="1">
-        <v>1217</v>
+        <v>1260</v>
       </c>
       <c r="M73" s="1">
-        <v>1499</v>
+        <v>1624</v>
       </c>
       <c r="N73" s="1">
-        <v>1450</v>
+        <v>1516</v>
       </c>
       <c r="O73" s="1">
-        <v>1475</v>
+        <v>1393</v>
       </c>
       <c r="P73" s="1">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B74" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C74" s="1">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="D74" s="1">
-        <v>60</v>
+        <v>195</v>
       </c>
       <c r="E74" s="1">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="F74" s="1">
-        <v>425</v>
+        <v>346</v>
       </c>
       <c r="G74" s="1">
-        <v>466</v>
+        <v>503</v>
       </c>
       <c r="H74" s="1">
-        <v>601</v>
+        <v>650</v>
       </c>
       <c r="I74" s="1">
         <v>812</v>
       </c>
       <c r="J74" s="1">
-        <v>928</v>
+        <v>695</v>
       </c>
       <c r="K74" s="1">
-        <v>1082</v>
+        <v>1053</v>
       </c>
       <c r="L74" s="1">
-        <v>1200</v>
+        <v>1085</v>
       </c>
       <c r="M74" s="1">
-        <v>1437</v>
+        <v>1584</v>
       </c>
       <c r="N74" s="1">
-        <v>1487</v>
+        <v>1613</v>
       </c>
       <c r="O74" s="1">
-        <v>1397</v>
+        <v>1495</v>
       </c>
       <c r="P74" s="1">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B75" s="1">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C75" s="1">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D75" s="1">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="E75" s="1">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="F75" s="1">
-        <v>419</v>
+        <v>287</v>
       </c>
       <c r="G75" s="1">
-        <v>477</v>
+        <v>515</v>
       </c>
       <c r="H75" s="1">
-        <v>580</v>
+        <v>681</v>
       </c>
       <c r="I75" s="1">
-        <v>776</v>
+        <v>806</v>
       </c>
       <c r="J75" s="1">
-        <v>1007</v>
+        <v>828</v>
       </c>
       <c r="K75" s="1">
-        <v>1170</v>
+        <v>1025</v>
       </c>
       <c r="L75" s="1">
-        <v>1019</v>
+        <v>1217</v>
       </c>
       <c r="M75" s="1">
-        <v>1798</v>
+        <v>1499</v>
       </c>
       <c r="N75" s="1">
-        <v>1245</v>
+        <v>1450</v>
       </c>
       <c r="O75" s="1">
-        <v>1431</v>
+        <v>1475</v>
       </c>
       <c r="P75" s="1">
-        <v>2033</v>
-      </c>
-    </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B76" s="1">
         <v>36</v>
       </c>
       <c r="C76" s="1">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D76" s="1">
-        <v>183</v>
+        <v>60</v>
       </c>
       <c r="E76" s="1">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F76" s="1">
-        <v>351</v>
+        <v>425</v>
       </c>
       <c r="G76" s="1">
-        <v>621</v>
+        <v>466</v>
       </c>
       <c r="H76" s="1">
-        <v>613</v>
+        <v>601</v>
       </c>
       <c r="I76" s="1">
-        <v>748</v>
+        <v>812</v>
       </c>
       <c r="J76" s="1">
-        <v>946</v>
+        <v>928</v>
       </c>
       <c r="K76" s="1">
-        <v>981</v>
+        <v>1082</v>
       </c>
       <c r="L76" s="1">
-        <v>1011</v>
+        <v>1200</v>
       </c>
       <c r="M76" s="1">
-        <v>1405</v>
+        <v>1437</v>
       </c>
       <c r="N76" s="1">
-        <v>1493</v>
+        <v>1487</v>
       </c>
       <c r="O76" s="1">
-        <v>1442</v>
+        <v>1397</v>
       </c>
       <c r="P76" s="1">
-        <v>2071</v>
-      </c>
-    </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B77" s="1">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C77" s="1">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D77" s="1">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="E77" s="1">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="F77" s="1">
-        <v>280</v>
+        <v>419</v>
       </c>
       <c r="G77" s="1">
-        <v>503</v>
+        <v>477</v>
       </c>
       <c r="H77" s="1">
-        <v>693</v>
+        <v>580</v>
       </c>
       <c r="I77" s="1">
-        <v>702</v>
+        <v>776</v>
       </c>
       <c r="J77" s="1">
-        <v>818</v>
+        <v>1007</v>
       </c>
       <c r="K77" s="1">
-        <v>1017</v>
+        <v>1170</v>
       </c>
       <c r="L77" s="1">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="M77" s="1">
-        <v>1903</v>
+        <v>1798</v>
       </c>
       <c r="N77" s="1">
-        <v>1194</v>
+        <v>1245</v>
       </c>
       <c r="O77" s="1">
-        <v>1449</v>
+        <v>1431</v>
       </c>
       <c r="P77" s="1">
-        <v>1963</v>
-      </c>
-    </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B78" s="1">
         <v>36</v>
       </c>
       <c r="C78" s="1">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D78" s="1">
-        <v>66</v>
+        <v>183</v>
       </c>
       <c r="E78" s="1">
-        <v>191</v>
+        <v>147</v>
       </c>
       <c r="F78" s="1">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="G78" s="1">
-        <v>467</v>
+        <v>621</v>
       </c>
       <c r="H78" s="1">
-        <v>669</v>
+        <v>613</v>
       </c>
       <c r="I78" s="1">
-        <v>733</v>
+        <v>748</v>
       </c>
       <c r="J78" s="1">
-        <v>1058</v>
+        <v>946</v>
       </c>
       <c r="K78" s="1">
-        <v>962</v>
+        <v>981</v>
       </c>
       <c r="L78" s="1">
-        <v>999</v>
+        <v>1011</v>
       </c>
       <c r="M78" s="1">
-        <v>1801</v>
+        <v>1405</v>
       </c>
       <c r="N78" s="1">
-        <v>1330</v>
+        <v>1493</v>
       </c>
       <c r="O78" s="1">
-        <v>1452</v>
+        <v>1442</v>
       </c>
       <c r="P78" s="1">
-        <v>2119</v>
-      </c>
-    </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B79" s="1">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C79" s="1">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D79" s="1">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="E79" s="1">
-        <v>99</v>
+        <v>172</v>
       </c>
       <c r="F79" s="1">
-        <v>383</v>
+        <v>280</v>
       </c>
       <c r="G79" s="1">
-        <v>534</v>
+        <v>503</v>
       </c>
       <c r="H79" s="1">
-        <v>610</v>
+        <v>693</v>
       </c>
       <c r="I79" s="1">
-        <v>805</v>
+        <v>702</v>
       </c>
       <c r="J79" s="1">
-        <v>937</v>
+        <v>818</v>
       </c>
       <c r="K79" s="1">
-        <v>934</v>
+        <v>1017</v>
       </c>
       <c r="L79" s="1">
-        <v>1121</v>
+        <v>1022</v>
       </c>
       <c r="M79" s="1">
         <v>1775</v>
       </c>
       <c r="N79" s="1">
-        <v>1264</v>
+        <v>1194</v>
       </c>
       <c r="O79" s="1">
-        <v>1520</v>
+        <v>1449</v>
       </c>
       <c r="P79" s="1">
-        <v>1949</v>
-      </c>
-    </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B80" s="1">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C80" s="1">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D80" s="1">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="E80" s="1">
-        <v>120</v>
+        <v>191</v>
       </c>
       <c r="F80" s="1">
-        <v>422</v>
+        <v>333</v>
       </c>
       <c r="G80" s="1">
-        <v>429</v>
+        <v>467</v>
       </c>
       <c r="H80" s="1">
-        <v>712</v>
+        <v>669</v>
       </c>
       <c r="I80" s="1">
-        <v>928</v>
+        <v>733</v>
       </c>
       <c r="J80" s="1">
-        <v>1017</v>
+        <v>1058</v>
       </c>
       <c r="K80" s="1">
-        <v>955</v>
+        <v>962</v>
       </c>
       <c r="L80" s="1">
-        <v>1016</v>
+        <v>999</v>
       </c>
       <c r="M80" s="1">
-        <v>1809</v>
+        <v>1569</v>
       </c>
       <c r="N80" s="1">
-        <v>1205</v>
+        <v>1330</v>
       </c>
       <c r="O80" s="1">
-        <v>1376</v>
+        <v>1452</v>
       </c>
       <c r="P80" s="1">
-        <v>2072</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="81" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B81" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C81" s="1">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D81" s="1">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E81" s="1">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F81" s="1">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="G81" s="1">
-        <v>499</v>
+        <v>534</v>
       </c>
       <c r="H81" s="1">
-        <v>545</v>
+        <v>610</v>
       </c>
       <c r="I81" s="1">
-        <v>840</v>
+        <v>805</v>
       </c>
       <c r="J81" s="1">
-        <v>985</v>
+        <v>937</v>
       </c>
       <c r="K81" s="1">
-        <v>956</v>
+        <v>934</v>
       </c>
       <c r="L81" s="1">
-        <v>1256</v>
+        <v>1121</v>
       </c>
       <c r="M81" s="1">
-        <v>1847</v>
+        <v>1729</v>
       </c>
       <c r="N81" s="1">
-        <v>1252</v>
+        <v>1264</v>
       </c>
       <c r="O81" s="1">
-        <v>1370</v>
+        <v>1520</v>
       </c>
       <c r="P81" s="1">
-        <v>2073</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="82" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C82" s="1">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D82" s="1">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E82" s="1">
-        <v>177</v>
+        <v>120</v>
       </c>
       <c r="F82" s="1">
-        <v>212</v>
+        <v>422</v>
       </c>
       <c r="G82" s="1">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="H82" s="1">
-        <v>597</v>
+        <v>712</v>
       </c>
       <c r="I82" s="1">
-        <v>745</v>
+        <v>928</v>
       </c>
       <c r="J82" s="1">
-        <v>837</v>
+        <v>1017</v>
       </c>
       <c r="K82" s="1">
-        <v>1001</v>
+        <v>955</v>
       </c>
       <c r="L82" s="1">
-        <v>1103</v>
+        <v>1016</v>
       </c>
       <c r="M82" s="1">
-        <v>1846</v>
+        <v>1784</v>
       </c>
       <c r="N82" s="1">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="O82" s="1">
-        <v>1400</v>
+        <v>1376</v>
       </c>
       <c r="P82" s="1">
-        <v>1971</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.25">
@@ -10216,304 +10243,307 @@
         <v>37</v>
       </c>
       <c r="C83" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D83" s="1">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E83" s="1">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="F83" s="1">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="G83" s="1">
-        <v>456</v>
+        <v>499</v>
       </c>
       <c r="H83" s="1">
-        <v>610</v>
+        <v>545</v>
       </c>
       <c r="I83" s="1">
-        <v>581</v>
+        <v>840</v>
       </c>
       <c r="J83" s="1">
-        <v>1049</v>
+        <v>985</v>
       </c>
       <c r="K83" s="1">
-        <v>983</v>
+        <v>956</v>
       </c>
       <c r="L83" s="1">
-        <v>1253</v>
+        <v>1256</v>
       </c>
       <c r="M83" s="1">
-        <v>1569</v>
+        <v>1465</v>
       </c>
       <c r="N83" s="1">
-        <v>1244</v>
+        <v>1252</v>
       </c>
       <c r="O83" s="1">
-        <v>1364</v>
+        <v>1370</v>
       </c>
       <c r="P83" s="1">
-        <v>2072</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B84" s="1">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C84" s="1">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D84" s="1">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="E84" s="1">
-        <v>102</v>
+        <v>177</v>
       </c>
       <c r="F84" s="1">
-        <v>320</v>
+        <v>212</v>
       </c>
       <c r="G84" s="1">
-        <v>532</v>
+        <v>452</v>
       </c>
       <c r="H84" s="1">
-        <v>535</v>
+        <v>597</v>
       </c>
       <c r="I84" s="1">
-        <v>665</v>
+        <v>745</v>
       </c>
       <c r="J84" s="1">
-        <v>936</v>
+        <v>837</v>
       </c>
       <c r="K84" s="1">
-        <v>995</v>
+        <v>1001</v>
       </c>
       <c r="L84" s="1">
         <v>1103</v>
       </c>
-      <c r="M84" s="1">
-        <v>1729</v>
-      </c>
       <c r="N84" s="1">
-        <v>1213</v>
+        <v>1204</v>
       </c>
       <c r="O84" s="1">
-        <v>1474</v>
+        <v>1400</v>
       </c>
       <c r="P84" s="1">
-        <v>2172</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C85" s="1">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D85" s="1">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="E85" s="1">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="F85" s="1">
-        <v>186</v>
+        <v>356</v>
       </c>
       <c r="G85" s="1">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="H85" s="1">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="I85" s="1">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="J85" s="1">
-        <v>961</v>
+        <v>1049</v>
       </c>
       <c r="K85" s="1">
-        <v>1021</v>
+        <v>983</v>
       </c>
       <c r="L85" s="1">
-        <v>1021</v>
-      </c>
-      <c r="M85" s="1">
-        <v>1784</v>
+        <v>1253</v>
       </c>
       <c r="N85" s="1">
-        <v>1068</v>
+        <v>1244</v>
       </c>
       <c r="O85" s="1">
-        <v>1422</v>
+        <v>1364</v>
       </c>
       <c r="P85" s="1">
-        <v>2069</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="86" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C86" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D86" s="1">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="E86" s="1">
-        <v>211</v>
+        <v>102</v>
       </c>
       <c r="F86" s="1">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="G86" s="1">
-        <v>313</v>
+        <v>532</v>
       </c>
       <c r="H86" s="1">
-        <v>671</v>
+        <v>535</v>
       </c>
       <c r="I86" s="1">
-        <v>720</v>
+        <v>665</v>
       </c>
       <c r="J86" s="1">
-        <v>982</v>
+        <v>936</v>
       </c>
       <c r="K86" s="1">
-        <v>972</v>
+        <v>995</v>
       </c>
       <c r="L86" s="1">
-        <v>1023</v>
-      </c>
-      <c r="M86" s="1">
-        <v>1465</v>
+        <v>1103</v>
       </c>
       <c r="N86" s="1">
-        <v>1189</v>
+        <v>1213</v>
       </c>
       <c r="O86" s="1">
-        <v>1384</v>
+        <v>1474</v>
       </c>
       <c r="P86" s="1">
-        <v>2248</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="87" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C87" s="1">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D87" s="1">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E87" s="1">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="F87" s="1">
-        <v>342</v>
+        <v>186</v>
       </c>
       <c r="G87" s="1">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="H87" s="1">
-        <v>577</v>
+        <v>623</v>
       </c>
       <c r="I87" s="1">
-        <v>575</v>
+        <v>559</v>
+      </c>
+      <c r="J87" s="1">
+        <v>961</v>
       </c>
       <c r="K87" s="1">
-        <v>1010</v>
+        <v>1021</v>
       </c>
       <c r="L87" s="1">
-        <v>1059</v>
+        <v>1021</v>
       </c>
       <c r="N87" s="1">
-        <v>1188</v>
+        <v>1068</v>
       </c>
       <c r="O87" s="1">
-        <v>1445</v>
+        <v>1422</v>
       </c>
       <c r="P87" s="1">
-        <v>2536</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="88" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
+        <v>46</v>
+      </c>
+      <c r="C88" s="1">
         <v>36</v>
       </c>
-      <c r="C88" s="1">
-        <v>35</v>
-      </c>
       <c r="D88" s="1">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E88" s="1">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="F88" s="1">
-        <v>317</v>
+        <v>344</v>
       </c>
       <c r="G88" s="1">
-        <v>501</v>
+        <v>313</v>
       </c>
       <c r="H88" s="1">
-        <v>580</v>
+        <v>671</v>
       </c>
       <c r="I88" s="1">
-        <v>712</v>
+        <v>720</v>
+      </c>
+      <c r="J88" s="1">
+        <v>982</v>
       </c>
       <c r="K88" s="1">
-        <v>967</v>
+        <v>972</v>
       </c>
       <c r="L88" s="1">
-        <v>1077</v>
+        <v>1023</v>
       </c>
       <c r="N88" s="1">
-        <v>1418</v>
+        <v>1189</v>
       </c>
       <c r="O88" s="1">
-        <v>1418</v>
+        <v>1384</v>
+      </c>
+      <c r="P88" s="1">
+        <v>2248</v>
       </c>
     </row>
     <row r="89" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B89" s="1">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C89" s="1">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D89" s="1">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E89" s="1">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F89" s="1">
-        <v>230</v>
+        <v>342</v>
       </c>
       <c r="G89" s="1">
-        <v>431</v>
+        <v>487</v>
       </c>
       <c r="H89" s="1">
-        <v>612</v>
+        <v>577</v>
       </c>
       <c r="I89" s="1">
-        <v>701</v>
+        <v>575</v>
       </c>
       <c r="K89" s="1">
-        <v>978</v>
+        <v>1010</v>
       </c>
       <c r="L89" s="1">
-        <v>1220</v>
+        <v>1059</v>
       </c>
       <c r="N89" s="1">
-        <v>1270</v>
+        <v>1188</v>
       </c>
       <c r="O89" s="1">
-        <v>1382</v>
+        <v>1445</v>
+      </c>
+      <c r="P89" s="1">
+        <v>2536</v>
       </c>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.25">
@@ -10521,208 +10551,284 @@
         <v>36</v>
       </c>
       <c r="C90" s="1">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D90" s="1">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E90" s="1">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="F90" s="1">
-        <v>193</v>
+        <v>317</v>
       </c>
       <c r="G90" s="1">
-        <v>484</v>
+        <v>501</v>
       </c>
       <c r="H90" s="1">
-        <v>599</v>
+        <v>580</v>
       </c>
       <c r="I90" s="1">
-        <v>788</v>
+        <v>712</v>
       </c>
       <c r="K90" s="1">
-        <v>1007</v>
+        <v>967</v>
       </c>
       <c r="L90" s="1">
-        <v>1132</v>
+        <v>1077</v>
       </c>
       <c r="N90" s="1">
-        <v>1280</v>
+        <v>1418</v>
       </c>
       <c r="O90" s="1">
-        <v>1343</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="91" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B91" s="1">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C91" s="1">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D91" s="1">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="E91" s="1">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="F91" s="1">
-        <v>187</v>
+        <v>230</v>
       </c>
       <c r="G91" s="1">
-        <v>463</v>
+        <v>431</v>
       </c>
       <c r="H91" s="1">
-        <v>624</v>
+        <v>612</v>
       </c>
       <c r="I91" s="1">
-        <v>782</v>
+        <v>701</v>
       </c>
       <c r="K91" s="1">
-        <v>984</v>
+        <v>978</v>
       </c>
       <c r="L91" s="1">
-        <v>1215</v>
+        <v>1220</v>
       </c>
       <c r="N91" s="1">
-        <v>1265</v>
+        <v>1270</v>
       </c>
       <c r="O91" s="1">
-        <v>1301</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="92" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C92" s="1">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D92" s="1">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E92" s="1">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="F92" s="1">
-        <v>350</v>
+        <v>193</v>
       </c>
       <c r="G92" s="1">
-        <v>439</v>
+        <v>484</v>
       </c>
       <c r="H92" s="1">
-        <v>633</v>
+        <v>599</v>
       </c>
       <c r="I92" s="1">
-        <v>833</v>
+        <v>788</v>
+      </c>
+      <c r="K92" s="1">
+        <v>1007</v>
       </c>
       <c r="L92" s="1">
-        <v>1170</v>
+        <v>1132</v>
       </c>
       <c r="N92" s="1">
-        <v>1295</v>
+        <v>1280</v>
       </c>
       <c r="O92" s="1">
-        <v>1491</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="93" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B93" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C93" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D93" s="1">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="E93" s="1">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="F93" s="1">
-        <v>414</v>
+        <v>187</v>
       </c>
       <c r="G93" s="1">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="H93" s="1">
-        <v>560</v>
+        <v>624</v>
       </c>
       <c r="I93" s="1">
-        <v>733</v>
+        <v>782</v>
+      </c>
+      <c r="K93" s="1">
+        <v>984</v>
       </c>
       <c r="L93" s="1">
-        <v>1288</v>
+        <v>1215</v>
       </c>
       <c r="N93" s="1">
-        <v>1384</v>
+        <v>1265</v>
       </c>
       <c r="O93" s="1">
-        <v>1390</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="94" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C94" s="1">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D94" s="1">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E94" s="1">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="F94" s="1">
-        <v>403</v>
+        <v>350</v>
       </c>
       <c r="G94" s="1">
-        <v>411</v>
+        <v>439</v>
       </c>
       <c r="H94" s="1">
-        <v>601</v>
+        <v>633</v>
       </c>
       <c r="I94" s="1">
-        <v>817</v>
+        <v>833</v>
+      </c>
+      <c r="L94" s="1">
+        <v>1170</v>
       </c>
       <c r="N94" s="1">
-        <v>1267</v>
+        <v>1295</v>
       </c>
       <c r="O94" s="1">
-        <v>1518</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="95" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
+        <v>43</v>
+      </c>
+      <c r="C95" s="1">
+        <v>45</v>
+      </c>
+      <c r="D95" s="1">
+        <v>55</v>
+      </c>
+      <c r="E95" s="1">
+        <v>92</v>
+      </c>
+      <c r="F95" s="1">
+        <v>414</v>
+      </c>
+      <c r="G95" s="1">
+        <v>478</v>
+      </c>
+      <c r="H95" s="1">
+        <v>560</v>
+      </c>
+      <c r="I95" s="1">
+        <v>733</v>
+      </c>
+      <c r="L95" s="1">
+        <v>1288</v>
+      </c>
+      <c r="N95" s="1">
+        <v>1384</v>
+      </c>
+      <c r="O95" s="1">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B96" s="1">
+        <v>37</v>
+      </c>
+      <c r="C96" s="1">
+        <v>31</v>
+      </c>
+      <c r="D96" s="1">
+        <v>73</v>
+      </c>
+      <c r="E96" s="1">
+        <v>101</v>
+      </c>
+      <c r="F96" s="1">
+        <v>403</v>
+      </c>
+      <c r="G96" s="1">
+        <v>411</v>
+      </c>
+      <c r="H96" s="1">
+        <v>601</v>
+      </c>
+      <c r="I96" s="1">
+        <v>817</v>
+      </c>
+      <c r="N96" s="1">
+        <v>1267</v>
+      </c>
+      <c r="O96" s="1">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B97" s="1">
         <v>24</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C97" s="1">
         <v>34</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D97" s="1">
         <v>87</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E97" s="1">
         <v>141</v>
       </c>
-      <c r="F95" s="1">
+      <c r="F97" s="1">
         <v>421</v>
       </c>
-      <c r="G95" s="1">
+      <c r="G97" s="1">
         <v>487</v>
       </c>
-      <c r="H95" s="1">
+      <c r="H97" s="1">
         <v>816</v>
       </c>
-      <c r="I95" s="1">
+      <c r="I97" s="1">
         <v>875</v>
       </c>
-      <c r="N95" s="1">
+      <c r="N97" s="1">
         <v>1277</v>
       </c>
-      <c r="O95" s="1">
+      <c r="O97" s="1">
         <v>1432</v>
       </c>
     </row>
@@ -10735,8 +10841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>